<commit_message>
fix bug #29815 #29786 #29787
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KMR004_Detail.xlsx
+++ b/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KMR004_Detail.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -446,11 +446,11 @@
   </sheetPr>
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="10.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="10.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.11"/>
@@ -528,11 +528,11 @@
   </sheetPr>
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3"/>
@@ -632,9 +632,20 @@
       <c r="K7" s="29"/>
       <c r="L7" s="29"/>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" customFormat="false" ht="8.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B8:E8"/>
+  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
uk/release_pj/lunch_order_1162: update QA #121252
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KMR004_Detail.xlsx
+++ b/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KMR004_Detail.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Nittsu\Project\UniversalK\nts.uk\uk.at\at.file\nts.uk.file.at.infra\src\main\resources\report\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UK Source\UK Source 5\nts.uk\uk.at\at.file\nts.uk.file.at.infra\src\main\resources\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F950D514-EFE5-48D6-9249-7C882726F8D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6">
     <font>
       <sz val="11"/>
@@ -289,97 +288,106 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="標準 3" xfId="1" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="標準 3" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -758,11 +766,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -782,52 +790,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="2"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
+      <c r="A1" s="30"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="29"/>
     </row>
     <row r="2" spans="1:10" ht="11.85" customHeight="1">
-      <c r="A2" s="2"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
+      <c r="A2" s="30"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="29"/>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="2"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
+      <c r="A3" s="1"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
     </row>
     <row r="4" spans="1:10" ht="8.25" customHeight="1"/>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:J1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:J2"/>
-    <mergeCell ref="B3:E3"/>
+  <mergeCells count="2">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:I2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
@@ -837,109 +842,109 @@
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="A1" s="3"/>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
+      <c r="A1" s="2"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
     </row>
     <row r="2" spans="1:12">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
     </row>
     <row r="3" spans="1:12">
-      <c r="A3" s="9"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="11"/>
-      <c r="L3" s="14"/>
+      <c r="A3" s="8"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="13"/>
     </row>
     <row r="4" spans="1:12">
-      <c r="A4" s="15"/>
-      <c r="B4" s="15"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="15"/>
-      <c r="J4" s="15"/>
-      <c r="K4" s="15"/>
-      <c r="L4" s="17"/>
+      <c r="A4" s="14"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="16"/>
     </row>
     <row r="5" spans="1:12">
-      <c r="A5" s="18"/>
-      <c r="B5" s="19"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="19"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="21"/>
-      <c r="J5" s="19"/>
-      <c r="K5" s="19"/>
-      <c r="L5" s="22"/>
+      <c r="A5" s="17"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="18"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="21"/>
     </row>
     <row r="6" spans="1:12">
-      <c r="A6" s="23"/>
-      <c r="B6" s="23"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="25"/>
-      <c r="I6" s="23"/>
-      <c r="J6" s="23"/>
-      <c r="K6" s="23"/>
-      <c r="L6" s="25"/>
+      <c r="A6" s="22"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="22"/>
+      <c r="J6" s="22"/>
+      <c r="K6" s="22"/>
+      <c r="L6" s="24"/>
     </row>
     <row r="7" spans="1:12">
-      <c r="A7" s="26"/>
-      <c r="B7" s="27"/>
-      <c r="C7" s="27"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="27"/>
-      <c r="I7" s="29"/>
-      <c r="J7" s="29"/>
-      <c r="K7" s="29"/>
-      <c r="L7" s="29"/>
+      <c r="A7" s="25"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26"/>
+      <c r="I7" s="28"/>
+      <c r="J7" s="28"/>
+      <c r="K7" s="28"/>
+      <c r="L7" s="28"/>
     </row>
     <row r="8" spans="1:12">
-      <c r="A8" s="2"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
+      <c r="A8" s="1"/>
+      <c r="B8" s="32"/>
+      <c r="C8" s="32"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="32"/>
     </row>
     <row r="9" spans="1:12" ht="8.25" customHeight="1"/>
     <row r="10" spans="1:12" ht="13.9" customHeight="1"/>

</xml_diff>